<commit_message>
fixing item list number
</commit_message>
<xml_diff>
--- a/Purchasing List.xlsx
+++ b/Purchasing List.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HAL9000/Dropbox (MIT)/DesktopMuonDetector/CosmicWatch/Detector_Versions/CosmicWatcher_MIT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HAL9000/Dropbox (MIT)/DesktopMuonDetector/CosmicWatch/GitHub/CosmicWatch-Desktop-Muon-Detector-v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6260" yWindow="440" windowWidth="28240" windowHeight="19420" tabRatio="500"/>
+    <workbookView xWindow="5360" yWindow="440" windowWidth="28240" windowHeight="19420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -350,9 +350,6 @@
     <t>Detector Purchasing List</t>
   </si>
   <si>
-    <t>Case Purchasing List</t>
-  </si>
-  <si>
     <t>Non-Inverting Buffer</t>
   </si>
   <si>
@@ -522,6 +519,9 @@
   </si>
   <si>
     <t>https://www.amazon.com/uxcell-Phone-Memory-Holder-Sockets/dp/B01AHYS7K8/ref=sr_1_1?ie=UTF8&amp;qid=1515421217&amp;sr=8-1&amp;keywords=uxcell+6+Pcs+SMT+SMDs682/141132599560?epid=1171059511&amp;hash=item20dc289108:g:qRkAAOxypNtSnqd3)</t>
+  </si>
+  <si>
+    <t>Enclosure Purchasing List</t>
   </si>
 </sst>
 </file>
@@ -733,7 +733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -776,9 +776,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -859,9 +856,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1165,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="114" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1180,51 +1174,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" s="21"/>
+      <c r="B1" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="56"/>
+      <c r="C3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="54"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="F6" s="58"/>
-      <c r="G6" s="22"/>
+      <c r="B6" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="56"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="21"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="22"/>
+      <c r="B7" s="20"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
@@ -1261,25 +1255,25 @@
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D10" s="9">
         <v>5</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="22">
         <f>0.0071*D10</f>
         <v>3.5500000000000004E-2</v>
       </c>
       <c r="F10" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>147</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>45</v>
@@ -1287,7 +1281,7 @@
       <c r="D11" s="9">
         <v>4</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="22">
         <f>0.0088 *D11</f>
         <v>3.5200000000000002E-2</v>
       </c>
@@ -1300,28 +1294,28 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D12" s="9">
         <v>2</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="22">
         <f>0.0088 *D12</f>
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="F12" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>151</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>40</v>
@@ -1329,7 +1323,7 @@
       <c r="D13" s="9">
         <v>4</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="22">
         <f>0.0088 *D13</f>
         <v>3.5200000000000002E-2</v>
       </c>
@@ -1342,7 +1336,7 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>41</v>
@@ -1350,7 +1344,7 @@
       <c r="D14" s="9">
         <v>5</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="22">
         <f>0.0088*D14</f>
         <v>4.4000000000000004E-2</v>
       </c>
@@ -1363,28 +1357,28 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D15" s="9">
         <v>2</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="22">
         <f>0.0088 *D15</f>
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>42</v>
@@ -1392,7 +1386,7 @@
       <c r="D16" s="9">
         <v>3</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="22">
         <f>0.0088*D16</f>
         <v>2.64E-2</v>
       </c>
@@ -1405,7 +1399,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>43</v>
@@ -1413,7 +1407,7 @@
       <c r="D17" s="9">
         <v>2</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="22">
         <f>0.0088*D17</f>
         <v>1.7600000000000001E-2</v>
       </c>
@@ -1426,28 +1420,28 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="8">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D18" s="9">
         <v>2</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="22">
         <f>0.0267 *D18</f>
         <v>5.3400000000000003E-2</v>
       </c>
       <c r="F18" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>157</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>84</v>
@@ -1455,7 +1449,7 @@
       <c r="D19" s="9">
         <v>2</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="22">
         <f>0.0248 *D19</f>
         <v>4.9599999999999998E-2</v>
       </c>
@@ -1476,7 +1470,7 @@
       <c r="D20" s="9">
         <v>2</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="22">
         <f>0.1092 *D20</f>
         <v>0.21840000000000001</v>
       </c>
@@ -1489,28 +1483,28 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D21" s="8">
         <v>6</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="23">
         <f>0.0158*D21</f>
         <v>9.4800000000000009E-2</v>
       </c>
       <c r="F21" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>162</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="8">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>86</v>
@@ -1518,7 +1512,7 @@
       <c r="D22" s="9">
         <v>4</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="22">
         <f>0.0248*D22</f>
         <v>9.9199999999999997E-2</v>
       </c>
@@ -1531,7 +1525,7 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="8">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>87</v>
@@ -1539,7 +1533,7 @@
       <c r="D23" s="9">
         <v>3</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="22">
         <f>0.038*D23</f>
         <v>0.11399999999999999</v>
       </c>
@@ -1552,7 +1546,7 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="8">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>88</v>
@@ -1560,7 +1554,7 @@
       <c r="D24" s="9">
         <v>3</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="22">
         <f>0.0413*D24</f>
         <v>0.12390000000000001</v>
       </c>
@@ -1573,36 +1567,36 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="8">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D25" s="9">
         <v>2</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="22">
         <f>0.0536*D25</f>
         <v>0.1072</v>
       </c>
       <c r="F25" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="G25" s="10" t="s">
         <v>159</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="8">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D26" s="9">
         <v>1</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="22">
         <f>0.2226</f>
         <v>0.22259999999999999</v>
       </c>
@@ -1615,7 +1609,7 @@
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="8">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>57</v>
@@ -1623,7 +1617,7 @@
       <c r="D27" s="9">
         <v>2</v>
       </c>
-      <c r="E27" s="23">
+      <c r="E27" s="22">
         <f>0.1627 *2</f>
         <v>0.32540000000000002</v>
       </c>
@@ -1636,15 +1630,15 @@
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="8">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D28" s="9">
         <v>1</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="22">
         <f>0.4</f>
         <v>0.4</v>
       </c>
@@ -1657,7 +1651,7 @@
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="8">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>21</v>
@@ -1665,7 +1659,7 @@
       <c r="D29" s="9">
         <v>1</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="22">
         <f>0.4069</f>
         <v>0.40689999999999998</v>
       </c>
@@ -1678,7 +1672,7 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="8">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>49</v>
@@ -1686,7 +1680,7 @@
       <c r="D30" s="9">
         <v>1</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="22">
         <f>0.4509</f>
         <v>0.45090000000000002</v>
       </c>
@@ -1699,7 +1693,7 @@
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="8">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>14</v>
@@ -1707,7 +1701,7 @@
       <c r="D31" s="9">
         <v>1</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="22">
         <f>0.1862</f>
         <v>0.1862</v>
       </c>
@@ -1719,37 +1713,37 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="18">
-        <v>30</v>
-      </c>
-      <c r="C32" s="20" t="s">
+      <c r="B32" s="8">
+        <v>23</v>
+      </c>
+      <c r="C32" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="19">
-        <v>1</v>
-      </c>
-      <c r="E32" s="25">
+      <c r="D32" s="18">
+        <v>1</v>
+      </c>
+      <c r="E32" s="24">
         <f>0.8906</f>
         <v>0.89059999999999995</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="G32" s="19" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="8">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D33" s="9">
         <v>1</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="22">
         <f>1.6727</f>
         <v>1.6727000000000001</v>
       </c>
@@ -1762,28 +1756,28 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="8">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D34" s="9">
         <v>1</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="22">
         <f>0.1973</f>
         <v>0.1973</v>
       </c>
       <c r="F34" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="G34" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="11">
-        <v>21</v>
+      <c r="B35" s="8">
+        <v>26</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>61</v>
@@ -1791,7 +1785,7 @@
       <c r="D35" s="12">
         <v>2</v>
       </c>
-      <c r="E35" s="26">
+      <c r="E35" s="25">
         <f>0.33*2</f>
         <v>0.66</v>
       </c>
@@ -1803,8 +1797,8 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="11">
-        <v>22</v>
+      <c r="B36" s="8">
+        <v>27</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>103</v>
@@ -1812,7 +1806,7 @@
       <c r="D36" s="12">
         <v>4</v>
       </c>
-      <c r="E36" s="26">
+      <c r="E36" s="25">
         <f>9.01/100*4</f>
         <v>0.3604</v>
       </c>
@@ -1824,8 +1818,8 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="11">
-        <v>24</v>
+      <c r="B37" s="8">
+        <v>28</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>63</v>
@@ -1833,7 +1827,7 @@
       <c r="D37" s="12">
         <v>4</v>
       </c>
-      <c r="E37" s="26">
+      <c r="E37" s="25">
         <f>6.95/50*2</f>
         <v>0.27800000000000002</v>
       </c>
@@ -1845,8 +1839,8 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="14">
-        <v>25</v>
+      <c r="B38" s="8">
+        <v>29</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>97</v>
@@ -1854,7 +1848,7 @@
       <c r="D38" s="15">
         <v>1</v>
       </c>
-      <c r="E38" s="27">
+      <c r="E38" s="26">
         <v>2</v>
       </c>
       <c r="F38" s="16" t="s">
@@ -1865,8 +1859,8 @@
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="14">
-        <v>26</v>
+      <c r="B39" s="8">
+        <v>30</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>96</v>
@@ -1874,7 +1868,7 @@
       <c r="D39" s="15">
         <v>1</v>
       </c>
-      <c r="E39" s="27">
+      <c r="E39" s="26">
         <f>3.75</f>
         <v>3.75</v>
       </c>
@@ -1882,217 +1876,217 @@
         <v>13</v>
       </c>
       <c r="G39" s="17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B40" s="8">
+        <v>31</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="31">
+        <v>1</v>
+      </c>
+      <c r="E40" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="G40" s="33" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B40" s="31">
-        <v>26</v>
-      </c>
-      <c r="C40" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D40" s="32">
-        <v>1</v>
-      </c>
-      <c r="E40" s="33">
-        <v>0.25</v>
-      </c>
-      <c r="F40" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="G40" s="34" t="s">
-        <v>114</v>
-      </c>
-    </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="35">
-        <v>27</v>
-      </c>
-      <c r="C41" s="35" t="s">
+      <c r="B41" s="8">
+        <v>32</v>
+      </c>
+      <c r="C41" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="36">
-        <v>1</v>
-      </c>
-      <c r="E41" s="37">
+      <c r="D41" s="35">
+        <v>1</v>
+      </c>
+      <c r="E41" s="36">
         <f>5.54/50</f>
         <v>0.1108</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="G41" s="38" t="s">
-        <v>116</v>
+      <c r="G41" s="37" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B42" s="35">
-        <v>29</v>
-      </c>
-      <c r="C42" s="35" t="s">
+      <c r="B42" s="8">
+        <v>33</v>
+      </c>
+      <c r="C42" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="36">
-        <v>1</v>
-      </c>
-      <c r="E42" s="37">
+      <c r="D42" s="35">
+        <v>1</v>
+      </c>
+      <c r="E42" s="36">
         <v>2.246</v>
       </c>
-      <c r="F42" s="39" t="s">
+      <c r="F42" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="G42" s="40" t="s">
+      <c r="G42" s="39" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B43" s="35">
-        <v>27</v>
-      </c>
-      <c r="C43" s="35" t="s">
+      <c r="B43" s="8">
+        <v>34</v>
+      </c>
+      <c r="C43" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="36">
-        <v>1</v>
-      </c>
-      <c r="E43" s="37">
+      <c r="D43" s="35">
+        <v>1</v>
+      </c>
+      <c r="E43" s="36">
         <f>8.33/10</f>
         <v>0.83299999999999996</v>
       </c>
-      <c r="F43" s="35" t="s">
+      <c r="F43" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="G43" s="35" t="s">
+      <c r="G43" s="34" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B44" s="35">
-        <v>30</v>
-      </c>
-      <c r="C44" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="D44" s="36">
-        <v>1</v>
-      </c>
-      <c r="E44" s="37">
+      <c r="B44" s="8">
+        <v>35</v>
+      </c>
+      <c r="C44" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="35">
+        <v>1</v>
+      </c>
+      <c r="E44" s="36">
         <f>3.86/10</f>
         <v>0.38600000000000001</v>
       </c>
-      <c r="F44" s="39" t="s">
+      <c r="F44" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="G44" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="G44" s="39" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B45" s="35">
-        <v>30</v>
-      </c>
-      <c r="C45" s="39" t="s">
+      <c r="B45" s="8">
+        <v>36</v>
+      </c>
+      <c r="C45" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="36">
-        <v>1</v>
-      </c>
-      <c r="E45" s="37">
+      <c r="D45" s="35">
+        <v>1</v>
+      </c>
+      <c r="E45" s="36">
         <v>2.66</v>
       </c>
-      <c r="F45" s="39" t="s">
+      <c r="F45" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="G45" s="39" t="s">
+      <c r="G45" s="38" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B46" s="41">
-        <v>31</v>
-      </c>
-      <c r="C46" s="41" t="s">
+      <c r="B46" s="8">
+        <v>37</v>
+      </c>
+      <c r="C46" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="D46" s="42">
-        <v>1</v>
-      </c>
-      <c r="E46" s="43">
+      <c r="D46" s="41">
+        <v>1</v>
+      </c>
+      <c r="E46" s="42">
         <v>48</v>
       </c>
-      <c r="F46" s="41" t="s">
+      <c r="F46" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="G46" s="44" t="s">
+      <c r="G46" s="43" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B47" s="49">
-        <v>32</v>
-      </c>
-      <c r="C47" s="50" t="s">
+      <c r="B47" s="8">
+        <v>38</v>
+      </c>
+      <c r="C47" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="51">
-        <v>1</v>
-      </c>
-      <c r="E47" s="52">
+      <c r="D47" s="49">
+        <v>1</v>
+      </c>
+      <c r="E47" s="50">
         <v>10</v>
       </c>
-      <c r="F47" s="53" t="s">
+      <c r="F47" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="G47" s="54" t="s">
-        <v>149</v>
+      <c r="G47" s="52" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B48" s="45">
-        <v>33</v>
-      </c>
-      <c r="C48" s="45" t="s">
+      <c r="B48" s="8">
+        <v>39</v>
+      </c>
+      <c r="C48" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="46">
-        <v>1</v>
-      </c>
-      <c r="E48" s="47">
+      <c r="D48" s="45">
+        <v>1</v>
+      </c>
+      <c r="E48" s="46">
         <f>9.5/10</f>
         <v>0.95</v>
       </c>
-      <c r="F48" s="48" t="s">
+      <c r="F48" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="G48" s="57" t="s">
+      <c r="G48" s="55" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="E49" s="29">
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E49" s="28">
         <f>SUM(E11:E48)</f>
         <v>78.290900000000008</v>
       </c>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
     </row>
     <row r="51" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
-        <v>108</v>
+        <v>165</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
@@ -2121,24 +2115,24 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="35">
-        <v>1</v>
-      </c>
-      <c r="C53" s="35" t="s">
+      <c r="B53" s="34">
+        <v>1</v>
+      </c>
+      <c r="C53" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="D53" s="36">
+      <c r="D53" s="35">
         <v>4</v>
       </c>
-      <c r="E53" s="37">
+      <c r="E53" s="36">
         <f>2.29/200*4</f>
         <v>4.58E-2</v>
       </c>
-      <c r="F53" s="39" t="s">
+      <c r="F53" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="G53" s="39" t="s">
-        <v>119</v>
+      <c r="G53" s="38" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.2">
@@ -2146,12 +2140,12 @@
         <v>2</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D54" s="1">
         <v>1</v>
       </c>
-      <c r="E54" s="30">
+      <c r="E54" s="29">
         <v>9.2799999999999994</v>
       </c>
       <c r="F54" s="2" t="s">
@@ -2162,71 +2156,71 @@
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B55" s="45">
+      <c r="B55" s="44">
         <v>3</v>
       </c>
-      <c r="C55" s="45" t="s">
+      <c r="C55" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="D55" s="46">
-        <v>1</v>
-      </c>
-      <c r="E55" s="47">
+      <c r="D55" s="45">
+        <v>1</v>
+      </c>
+      <c r="E55" s="46">
         <f>9.05/10</f>
         <v>0.90500000000000003</v>
       </c>
-      <c r="F55" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="G55" s="48" t="s">
+      <c r="F55" s="47" t="s">
         <v>129</v>
       </c>
+      <c r="G55" s="47" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B56" s="35">
+      <c r="B56" s="34">
         <v>4</v>
       </c>
-      <c r="C56" s="35" t="s">
+      <c r="C56" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="36">
-        <v>1</v>
-      </c>
-      <c r="E56" s="37">
+      <c r="D56" s="35">
+        <v>1</v>
+      </c>
+      <c r="E56" s="36">
         <f>7.7/50</f>
         <v>0.154</v>
       </c>
-      <c r="F56" s="39" t="s">
+      <c r="F56" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="G56" s="39" t="s">
+      <c r="G56" s="38" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="E57" s="29">
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E57" s="28">
         <f>SUM(E53:E56)</f>
         <v>10.384799999999998</v>
       </c>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="28"/>
-      <c r="E58" s="55"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="53"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
     </row>
     <row r="59" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B59" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
@@ -2253,187 +2247,187 @@
       </c>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B61" s="35">
-        <v>1</v>
-      </c>
-      <c r="C61" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="D61" s="35">
-        <v>1</v>
-      </c>
-      <c r="E61" s="59">
+      <c r="B61" s="34">
+        <v>1</v>
+      </c>
+      <c r="C61" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D61" s="34">
+        <v>1</v>
+      </c>
+      <c r="E61" s="57">
         <f>8.54/200</f>
         <v>4.2699999999999995E-2</v>
       </c>
-      <c r="F61" s="60" t="s">
+      <c r="F61" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="G61" s="39" t="s">
+      <c r="G61" s="38" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B62" s="35">
+      <c r="B62" s="34">
         <v>2</v>
       </c>
-      <c r="C62" s="35" t="s">
+      <c r="C62" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D62" s="35" t="s">
+      <c r="D62" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="E62" s="59">
+      <c r="E62" s="57">
         <f>8.95/10</f>
         <v>0.89499999999999991</v>
       </c>
-      <c r="F62" s="60" t="s">
+      <c r="F62" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="G62" s="39" t="s">
-        <v>139</v>
+      <c r="G62" s="38" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B63" s="35">
+      <c r="B63" s="34">
         <v>3</v>
       </c>
-      <c r="C63" s="35" t="s">
+      <c r="C63" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D63" s="35" t="s">
+      <c r="D63" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="E63" s="59">
+      <c r="E63" s="57">
         <f>4.47/20</f>
         <v>0.22349999999999998</v>
       </c>
-      <c r="F63" s="60" t="s">
+      <c r="F63" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="G63" s="39" t="s">
+      <c r="G63" s="38" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B64" s="35">
+      <c r="B64" s="34">
         <v>4</v>
       </c>
-      <c r="C64" s="35" t="s">
+      <c r="C64" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" s="34">
+        <v>1</v>
+      </c>
+      <c r="E64" s="57">
+        <v>3</v>
+      </c>
+      <c r="F64" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="D64" s="35">
-        <v>1</v>
-      </c>
-      <c r="E64" s="59">
-        <v>3</v>
-      </c>
-      <c r="F64" s="60" t="s">
+      <c r="G64" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="G64" s="61" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B65" s="35">
+      <c r="B65" s="34">
         <v>5</v>
       </c>
-      <c r="C65" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="D65" s="35">
-        <v>1</v>
-      </c>
-      <c r="E65" s="59">
+      <c r="C65" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D65" s="34">
+        <v>1</v>
+      </c>
+      <c r="E65" s="57">
         <f>8/2</f>
         <v>4</v>
       </c>
-      <c r="F65" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="G65" s="61" t="s">
-        <v>128</v>
+      <c r="F65" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="G65" s="59" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B66" s="35">
+      <c r="B66" s="34">
         <v>6</v>
       </c>
-      <c r="C66" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="D66" s="35">
-        <v>1</v>
-      </c>
-      <c r="E66" s="59">
+      <c r="C66" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D66" s="34">
+        <v>1</v>
+      </c>
+      <c r="E66" s="57">
         <f>5.96</f>
         <v>5.96</v>
       </c>
-      <c r="F66" s="60" t="s">
-        <v>138</v>
-      </c>
-      <c r="G66" s="61" t="s">
+      <c r="F66" s="58" t="s">
         <v>137</v>
       </c>
+      <c r="G66" s="59" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B67" s="21"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="62" t="s">
-        <v>124</v>
-      </c>
-      <c r="E67" s="29">
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="E67" s="28">
         <f>SUM(E61:E66)</f>
         <v>14.121200000000002</v>
       </c>
-      <c r="F67" s="21"/>
-      <c r="G67" s="21"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="20"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B68" s="21"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="21"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="21"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
     </row>
     <row r="70" spans="2:7" ht="19" x14ac:dyDescent="0.25">
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="63" t="s">
-        <v>124</v>
-      </c>
-      <c r="E70" s="64">
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="61" t="s">
+        <v>123</v>
+      </c>
+      <c r="E70" s="62">
         <f>E67+E57+E49</f>
         <v>102.79690000000001</v>
       </c>
-      <c r="F70" s="21"/>
-      <c r="G70" s="21"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
     </row>
     <row r="71" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B71" s="21"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="21"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="21"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="20"/>
     </row>
     <row r="72" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B72" s="21"/>
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="21"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
added 10nF cap to purchasing list
</commit_message>
<xml_diff>
--- a/Purchasing List.xlsx
+++ b/Purchasing List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="170">
   <si>
     <t>Link</t>
   </si>
@@ -522,6 +522,18 @@
   </si>
   <si>
     <t>Enclosure Purchasing List</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 50V X7R 0805</t>
+  </si>
+  <si>
+    <t>490-1664-1-ND</t>
+  </si>
+  <si>
+    <t>Digikey Part Number: 490-1664-1-ND</t>
+  </si>
+  <si>
+    <t>10nF capacitor</t>
   </si>
 </sst>
 </file>
@@ -1157,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G72"/>
+  <dimension ref="B1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="114" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="114" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1206,14 +1218,18 @@
         <v>125</v>
       </c>
       <c r="C5" s="20"/>
-      <c r="G5" s="21"/>
+      <c r="G5" s="56" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="20" t="s">
         <v>142</v>
       </c>
       <c r="F6" s="56"/>
-      <c r="G6" s="21"/>
+      <c r="G6" s="56" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="20"/>
@@ -1549,20 +1565,20 @@
         <v>15</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>88</v>
+        <v>169</v>
       </c>
       <c r="D24" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E24" s="22">
-        <f>0.0413*D24</f>
-        <v>0.12390000000000001</v>
+        <f>0.0335</f>
+        <v>3.3500000000000002E-2</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>10</v>
+        <v>166</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>34</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
@@ -1570,20 +1586,20 @@
         <v>16</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>144</v>
+        <v>88</v>
       </c>
       <c r="D25" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" s="22">
-        <f>0.0536*D25</f>
-        <v>0.1072</v>
+        <f>0.0413*D25</f>
+        <v>0.12390000000000001</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>158</v>
+        <v>10</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>159</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
@@ -1591,62 +1607,62 @@
         <v>17</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D26" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" s="22">
-        <f>0.2226</f>
-        <v>0.22259999999999999</v>
+        <f>0.0536*D26</f>
+        <v>0.1072</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>30</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="8">
         <v>18</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>57</v>
+      <c r="C27" s="8" t="s">
+        <v>141</v>
       </c>
       <c r="D27" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" s="22">
-        <f>0.1627 *2</f>
-        <v>0.32540000000000002</v>
+        <f>0.2226</f>
+        <v>0.22259999999999999</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="8">
         <v>19</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>117</v>
+      <c r="C28" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="D28" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="22">
-        <f>0.4</f>
-        <v>0.4</v>
+        <f>0.1627 *2</f>
+        <v>0.32540000000000002</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
@@ -1654,20 +1670,20 @@
         <v>20</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="D29" s="9">
         <v>1</v>
       </c>
       <c r="E29" s="22">
-        <f>0.4069</f>
-        <v>0.40689999999999998</v>
+        <f>0.4</f>
+        <v>0.4</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
@@ -1675,20 +1691,20 @@
         <v>21</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="D30" s="9">
         <v>1</v>
       </c>
       <c r="E30" s="22">
-        <f>0.4509</f>
-        <v>0.45090000000000002</v>
+        <f>0.4069</f>
+        <v>0.40689999999999998</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
@@ -1696,62 +1712,62 @@
         <v>22</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="D31" s="9">
         <v>1</v>
       </c>
       <c r="E31" s="22">
-        <f>0.1862</f>
-        <v>0.1862</v>
+        <f>0.4509</f>
+        <v>0.45090000000000002</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" s="8">
         <v>23</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="18">
-        <v>1</v>
-      </c>
-      <c r="E32" s="24">
-        <f>0.8906</f>
-        <v>0.89059999999999995</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>98</v>
+      <c r="C32" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="9">
+        <v>1</v>
+      </c>
+      <c r="E32" s="22">
+        <f>0.1862</f>
+        <v>0.1862</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="8">
         <v>24</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="D33" s="9">
-        <v>1</v>
-      </c>
-      <c r="E33" s="22">
-        <f>1.6727</f>
-        <v>1.6727000000000001</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>22</v>
+      <c r="C33" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="18">
+        <v>1</v>
+      </c>
+      <c r="E33" s="24">
+        <f>0.8906</f>
+        <v>0.89059999999999995</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
@@ -1759,41 +1775,41 @@
         <v>25</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="D34" s="9">
         <v>1</v>
       </c>
       <c r="E34" s="22">
-        <f>0.1973</f>
-        <v>0.1973</v>
+        <f>1.6727</f>
+        <v>1.6727000000000001</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>134</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="8">
         <v>26</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="12">
-        <v>2</v>
-      </c>
-      <c r="E35" s="25">
-        <f>0.33*2</f>
-        <v>0.66</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>83</v>
+      <c r="C35" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="9">
+        <v>1</v>
+      </c>
+      <c r="E35" s="22">
+        <f>0.1973</f>
+        <v>0.1973</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
@@ -1801,20 +1817,20 @@
         <v>27</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="D36" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E36" s="25">
-        <f>9.01/100*4</f>
-        <v>0.3604</v>
+        <f>0.33*2</f>
+        <v>0.66</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>104</v>
+        <v>62</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -1822,40 +1838,41 @@
         <v>28</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="D37" s="12">
         <v>4</v>
       </c>
       <c r="E37" s="25">
-        <f>6.95/50*2</f>
-        <v>0.27800000000000002</v>
+        <f>9.01/100*4</f>
+        <v>0.3604</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>65</v>
+        <v>104</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="8">
         <v>29</v>
       </c>
-      <c r="C38" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D38" s="15">
-        <v>1</v>
-      </c>
-      <c r="E38" s="26">
-        <v>2</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>12</v>
+      <c r="C38" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="12">
+        <v>4</v>
+      </c>
+      <c r="E38" s="25">
+        <f>6.95/50*2</f>
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
@@ -1863,61 +1880,60 @@
         <v>30</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D39" s="15">
         <v>1</v>
       </c>
       <c r="E39" s="26">
-        <f>3.75</f>
-        <v>3.75</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>46</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="8">
         <v>31</v>
       </c>
-      <c r="C40" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="31">
-        <v>1</v>
-      </c>
-      <c r="E40" s="32">
-        <v>0.25</v>
-      </c>
-      <c r="F40" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="G40" s="33" t="s">
-        <v>113</v>
+      <c r="C40" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="15">
+        <v>1</v>
+      </c>
+      <c r="E40" s="26">
+        <f>3.75</f>
+        <v>3.75</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="8">
         <v>32</v>
       </c>
-      <c r="C41" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="D41" s="35">
-        <v>1</v>
-      </c>
-      <c r="E41" s="36">
-        <f>5.54/50</f>
-        <v>0.1108</v>
-      </c>
-      <c r="F41" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="G41" s="37" t="s">
-        <v>115</v>
+      <c r="C41" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" s="31">
+        <v>1</v>
+      </c>
+      <c r="E41" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" s="33" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
@@ -1925,19 +1941,20 @@
         <v>33</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>16</v>
+        <v>89</v>
       </c>
       <c r="D42" s="35">
         <v>1</v>
       </c>
       <c r="E42" s="36">
-        <v>2.246</v>
-      </c>
-      <c r="F42" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="G42" s="39" t="s">
-        <v>93</v>
+        <f>5.54/50</f>
+        <v>0.1108</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="G42" s="37" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
@@ -1945,41 +1962,40 @@
         <v>34</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="D43" s="35">
         <v>1</v>
       </c>
       <c r="E43" s="36">
-        <f>8.33/10</f>
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="F43" s="34" t="s">
-        <v>101</v>
-      </c>
-      <c r="G43" s="34" t="s">
-        <v>102</v>
+        <v>2.246</v>
+      </c>
+      <c r="F43" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G43" s="39" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44" s="8">
         <v>35</v>
       </c>
-      <c r="C44" s="38" t="s">
-        <v>124</v>
+      <c r="C44" s="34" t="s">
+        <v>68</v>
       </c>
       <c r="D44" s="35">
         <v>1</v>
       </c>
       <c r="E44" s="36">
-        <f>3.86/10</f>
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="F44" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="G44" s="38" t="s">
-        <v>164</v>
+        <f>8.33/10</f>
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" s="34" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
@@ -1987,408 +2003,421 @@
         <v>36</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>58</v>
+        <v>124</v>
       </c>
       <c r="D45" s="35">
         <v>1</v>
       </c>
       <c r="E45" s="36">
-        <v>2.66</v>
+        <f>3.86/10</f>
+        <v>0.38600000000000001</v>
       </c>
       <c r="F45" s="38" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="G45" s="38" t="s">
-        <v>92</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46" s="8">
         <v>37</v>
       </c>
-      <c r="C46" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="41">
-        <v>1</v>
-      </c>
-      <c r="E46" s="42">
-        <v>48</v>
-      </c>
-      <c r="F46" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="G46" s="43" t="s">
-        <v>54</v>
+      <c r="C46" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" s="35">
+        <v>1</v>
+      </c>
+      <c r="E46" s="36">
+        <v>2.66</v>
+      </c>
+      <c r="F46" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="G46" s="38" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47" s="8">
         <v>38</v>
       </c>
-      <c r="C47" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="D47" s="49">
-        <v>1</v>
-      </c>
-      <c r="E47" s="50">
-        <v>10</v>
-      </c>
-      <c r="F47" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="G47" s="52" t="s">
-        <v>148</v>
+      <c r="C47" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="41">
+        <v>1</v>
+      </c>
+      <c r="E47" s="42">
+        <v>48</v>
+      </c>
+      <c r="F47" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="G47" s="43" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48" s="8">
         <v>39</v>
       </c>
-      <c r="C48" s="44" t="s">
+      <c r="C48" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="49">
+        <v>1</v>
+      </c>
+      <c r="E48" s="50">
+        <v>10</v>
+      </c>
+      <c r="F48" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="G48" s="52" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B49" s="8">
+        <v>40</v>
+      </c>
+      <c r="C49" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D48" s="45">
-        <v>1</v>
-      </c>
-      <c r="E48" s="46">
+      <c r="D49" s="45">
+        <v>1</v>
+      </c>
+      <c r="E49" s="46">
         <f>9.5/10</f>
         <v>0.95</v>
       </c>
-      <c r="F48" s="47" t="s">
+      <c r="F49" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="G48" s="55" t="s">
+      <c r="G49" s="55" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="E49" s="28">
-        <f>SUM(E11:E48)</f>
-        <v>78.290900000000008</v>
-      </c>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
+      <c r="D50" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50" s="28">
+        <f>SUM(E11:E49)</f>
+        <v>78.324399999999997</v>
+      </c>
       <c r="F50" s="20"/>
       <c r="G50" s="20"/>
     </row>
-    <row r="51" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B51" s="5" t="s">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+    </row>
+    <row r="52" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="B52" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B52" s="3" t="s">
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B53" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="F53" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="34">
-        <v>1</v>
-      </c>
-      <c r="C53" s="34" t="s">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B54" s="34">
+        <v>1</v>
+      </c>
+      <c r="C54" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="D53" s="35">
+      <c r="D54" s="35">
         <v>4</v>
       </c>
-      <c r="E53" s="36">
+      <c r="E54" s="36">
         <f>2.29/200*4</f>
         <v>4.58E-2</v>
       </c>
-      <c r="F53" s="38" t="s">
+      <c r="F54" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="G53" s="38" t="s">
+      <c r="G54" s="38" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B54" s="1">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B55" s="1">
         <v>2</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D54" s="1">
-        <v>1</v>
-      </c>
-      <c r="E54" s="29">
+      <c r="D55" s="1">
+        <v>1</v>
+      </c>
+      <c r="E55" s="29">
         <v>9.2799999999999994</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B55" s="44">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B56" s="44">
         <v>3</v>
       </c>
-      <c r="C55" s="44" t="s">
+      <c r="C56" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="D55" s="45">
-        <v>1</v>
-      </c>
-      <c r="E55" s="46">
+      <c r="D56" s="45">
+        <v>1</v>
+      </c>
+      <c r="E56" s="46">
         <f>9.05/10</f>
         <v>0.90500000000000003</v>
       </c>
-      <c r="F55" s="47" t="s">
+      <c r="F56" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="G55" s="47" t="s">
+      <c r="G56" s="47" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B56" s="34">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B57" s="34">
         <v>4</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="C57" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="35">
-        <v>1</v>
-      </c>
-      <c r="E56" s="36">
+      <c r="D57" s="35">
+        <v>1</v>
+      </c>
+      <c r="E57" s="36">
         <f>7.7/50</f>
         <v>0.154</v>
       </c>
-      <c r="F56" s="38" t="s">
+      <c r="F57" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="G56" s="38" t="s">
+      <c r="G57" s="38" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="E57" s="28">
-        <f>SUM(E53:E56)</f>
-        <v>10.384799999999998</v>
-      </c>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
-      <c r="D58" s="27"/>
-      <c r="E58" s="53"/>
+      <c r="D58" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E58" s="28">
+        <f>SUM(E54:E57)</f>
+        <v>10.384799999999998</v>
+      </c>
       <c r="F58" s="20"/>
       <c r="G58" s="20"/>
     </row>
-    <row r="59" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B59" s="5" t="s">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+    </row>
+    <row r="60" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="B60" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="6"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B61" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="4" t="s">
+      <c r="E61" s="3"/>
+      <c r="F61" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B61" s="34">
-        <v>1</v>
-      </c>
-      <c r="C61" s="34" t="s">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B62" s="34">
+        <v>1</v>
+      </c>
+      <c r="C62" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="D61" s="34">
-        <v>1</v>
-      </c>
-      <c r="E61" s="57">
+      <c r="D62" s="34">
+        <v>1</v>
+      </c>
+      <c r="E62" s="57">
         <f>8.54/200</f>
         <v>4.2699999999999995E-2</v>
       </c>
-      <c r="F61" s="58" t="s">
+      <c r="F62" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="G61" s="38" t="s">
+      <c r="G62" s="38" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B62" s="34">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B63" s="34">
         <v>2</v>
       </c>
-      <c r="C62" s="34" t="s">
+      <c r="C63" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="D62" s="34" t="s">
+      <c r="D63" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="E62" s="57">
+      <c r="E63" s="57">
         <f>8.95/10</f>
         <v>0.89499999999999991</v>
       </c>
-      <c r="F62" s="58" t="s">
+      <c r="F63" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="G62" s="38" t="s">
+      <c r="G63" s="38" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B63" s="34">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B64" s="34">
         <v>3</v>
       </c>
-      <c r="C63" s="34" t="s">
+      <c r="C64" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D63" s="34" t="s">
+      <c r="D64" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="E63" s="57">
+      <c r="E64" s="57">
         <f>4.47/20</f>
         <v>0.22349999999999998</v>
       </c>
-      <c r="F63" s="58" t="s">
+      <c r="F64" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="G63" s="38" t="s">
+      <c r="G64" s="38" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B64" s="34">
-        <v>4</v>
-      </c>
-      <c r="C64" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="D64" s="34">
-        <v>1</v>
-      </c>
-      <c r="E64" s="57">
-        <v>3</v>
-      </c>
-      <c r="F64" s="58" t="s">
-        <v>121</v>
-      </c>
-      <c r="G64" s="59" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B65" s="34">
+        <v>4</v>
+      </c>
+      <c r="C65" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="D65" s="34">
+        <v>1</v>
+      </c>
+      <c r="E65" s="57">
+        <v>3</v>
+      </c>
+      <c r="F65" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="G65" s="59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B66" s="34">
         <v>5</v>
       </c>
-      <c r="C65" s="34" t="s">
+      <c r="C66" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="D65" s="34">
-        <v>1</v>
-      </c>
-      <c r="E65" s="57">
+      <c r="D66" s="34">
+        <v>1</v>
+      </c>
+      <c r="E66" s="57">
         <f>8/2</f>
         <v>4</v>
       </c>
-      <c r="F65" s="58" t="s">
+      <c r="F66" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="G65" s="59" t="s">
+      <c r="G66" s="59" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B66" s="34">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B67" s="34">
         <v>6</v>
       </c>
-      <c r="C66" s="34" t="s">
+      <c r="C67" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="D66" s="34">
-        <v>1</v>
-      </c>
-      <c r="E66" s="57">
+      <c r="D67" s="34">
+        <v>1</v>
+      </c>
+      <c r="E67" s="57">
         <f>5.96</f>
         <v>5.96</v>
       </c>
-      <c r="F66" s="58" t="s">
+      <c r="F67" s="58" t="s">
         <v>137</v>
       </c>
-      <c r="G66" s="59" t="s">
+      <c r="G67" s="59" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B67" s="20"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="E67" s="28">
-        <f>SUM(E61:E66)</f>
-        <v>14.121200000000002</v>
-      </c>
-      <c r="F67" s="20"/>
-      <c r="G67" s="20"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B68" s="20"/>
       <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
+      <c r="D68" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="E68" s="28">
+        <f>SUM(E62:E67)</f>
+        <v>14.121200000000002</v>
+      </c>
       <c r="F68" s="20"/>
       <c r="G68" s="20"/>
     </row>
@@ -2400,24 +2429,24 @@
       <c r="F69" s="20"/>
       <c r="G69" s="20"/>
     </row>
-    <row r="70" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B70" s="20"/>
       <c r="C70" s="20"/>
-      <c r="D70" s="61" t="s">
-        <v>123</v>
-      </c>
-      <c r="E70" s="62">
-        <f>E67+E57+E49</f>
-        <v>102.79690000000001</v>
-      </c>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
       <c r="F70" s="20"/>
       <c r="G70" s="20"/>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B71" s="20"/>
       <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
+      <c r="D71" s="61" t="s">
+        <v>123</v>
+      </c>
+      <c r="E71" s="62">
+        <f>E68+E58+E50</f>
+        <v>102.8304</v>
+      </c>
       <c r="F71" s="20"/>
       <c r="G71" s="20"/>
     </row>
@@ -2429,13 +2458,21 @@
       <c r="F72" s="20"/>
       <c r="G72" s="20"/>
     </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B73" s="20"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="20"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G41" r:id="rId1"/>
-    <hyperlink ref="G64" r:id="rId2"/>
-    <hyperlink ref="G48" r:id="rId3"/>
-    <hyperlink ref="G66" r:id="rId4" display="https://www.amazon.com/dp/B0742CWDN8/ref=twister_B07429LJXQ?_encoding=UTF8&amp;psc=1"/>
-    <hyperlink ref="G65" r:id="rId5"/>
+    <hyperlink ref="G42" r:id="rId1"/>
+    <hyperlink ref="G65" r:id="rId2"/>
+    <hyperlink ref="G49" r:id="rId3"/>
+    <hyperlink ref="G67" r:id="rId4" display="https://www.amazon.com/dp/B0742CWDN8/ref=twister_B07429LJXQ?_encoding=UTF8&amp;psc=1"/>
+    <hyperlink ref="G66" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updating OLED code and standoff requirements
</commit_message>
<xml_diff>
--- a/Purchasing List.xlsx
+++ b/Purchasing List.xlsx
@@ -212,9 +212,6 @@
     <t>Standoff for SiPM PCB</t>
   </si>
   <si>
-    <t>1/8" Hex Size, 3/8" Length, 0-80 Thread Size</t>
-  </si>
-  <si>
     <t>Plastic scintillator screws</t>
   </si>
   <si>
@@ -275,9 +272,6 @@
     <t>https://www.amazon.com/Electrical-Tape-several-colors-Black/dp/B003ZWN5ZM/ref=sr_1_6?ie=UTF8&amp;qid=1490898934&amp;sr=8-6&amp;keywords=black+electrical+tape</t>
   </si>
   <si>
-    <t>McMasterCarr part number: 91780A027</t>
-  </si>
-  <si>
     <t>22pF capacitor</t>
   </si>
   <si>
@@ -534,6 +528,12 @@
   </si>
   <si>
     <t>10nF capacitor</t>
+  </si>
+  <si>
+    <t>McMasterCarr part number: 91780A029</t>
+  </si>
+  <si>
+    <t>1/8" Hex Size, 7/16"" Length, 0-80 Thread Size</t>
   </si>
 </sst>
 </file>
@@ -1171,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="114" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="114" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1187,20 +1187,20 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B1" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C1" s="20"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C2" s="20"/>
       <c r="F2" s="20"/>
     </row>
     <row r="3" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C3" s="20"/>
       <c r="F3" s="20"/>
@@ -1208,27 +1208,27 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C4" s="20"/>
       <c r="G4" s="21"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C5" s="20"/>
       <c r="G5" s="56" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="56" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
@@ -1238,7 +1238,7 @@
     </row>
     <row r="8" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1257,7 +1257,7 @@
         <v>44</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>19</v>
@@ -1271,7 +1271,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D10" s="9">
         <v>5</v>
@@ -1281,10 +1281,10 @@
         <v>3.5500000000000004E-2</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
@@ -1313,7 +1313,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D12" s="9">
         <v>2</v>
@@ -1323,10 +1323,10 @@
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
@@ -1376,7 +1376,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D15" s="9">
         <v>2</v>
@@ -1386,10 +1386,10 @@
         <v>1.7600000000000001E-2</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
@@ -1439,7 +1439,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D18" s="9">
         <v>2</v>
@@ -1449,10 +1449,10 @@
         <v>5.3400000000000003E-2</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
@@ -1460,7 +1460,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D19" s="9">
         <v>2</v>
@@ -1481,7 +1481,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D20" s="9">
         <v>2</v>
@@ -1502,7 +1502,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D21" s="8">
         <v>6</v>
@@ -1512,10 +1512,10 @@
         <v>9.4800000000000009E-2</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
@@ -1523,7 +1523,7 @@
         <v>13</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D22" s="9">
         <v>4</v>
@@ -1544,7 +1544,7 @@
         <v>14</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D23" s="9">
         <v>3</v>
@@ -1565,7 +1565,7 @@
         <v>15</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D24" s="9">
         <v>4</v>
@@ -1575,10 +1575,10 @@
         <v>3.3500000000000002E-2</v>
       </c>
       <c r="F24" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="G24" s="10" t="s">
         <v>166</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
@@ -1586,7 +1586,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D25" s="9">
         <v>3</v>
@@ -1607,7 +1607,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D26" s="9">
         <v>2</v>
@@ -1617,10 +1617,10 @@
         <v>0.1072</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
@@ -1628,7 +1628,7 @@
         <v>18</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D27" s="9">
         <v>1</v>
@@ -1670,7 +1670,7 @@
         <v>20</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D29" s="9">
         <v>1</v>
@@ -1754,7 +1754,7 @@
         <v>24</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D33" s="18">
         <v>1</v>
@@ -1764,10 +1764,10 @@
         <v>0.89059999999999995</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
@@ -1775,7 +1775,7 @@
         <v>25</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D34" s="9">
         <v>1</v>
@@ -1796,7 +1796,7 @@
         <v>26</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D35" s="9">
         <v>1</v>
@@ -1806,10 +1806,10 @@
         <v>0.1973</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
@@ -1827,10 +1827,10 @@
         <v>0.66</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>62</v>
+        <v>169</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>83</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
@@ -1838,7 +1838,7 @@
         <v>28</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D37" s="12">
         <v>4</v>
@@ -1848,10 +1848,10 @@
         <v>0.3604</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
@@ -1859,7 +1859,7 @@
         <v>29</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D38" s="12">
         <v>4</v>
@@ -1869,10 +1869,10 @@
         <v>0.27800000000000002</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
@@ -1880,7 +1880,7 @@
         <v>30</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D39" s="15">
         <v>1</v>
@@ -1900,7 +1900,7 @@
         <v>31</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D40" s="15">
         <v>1</v>
@@ -1913,7 +1913,7 @@
         <v>13</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
@@ -1921,7 +1921,7 @@
         <v>32</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D41" s="31">
         <v>1</v>
@@ -1930,10 +1930,10 @@
         <v>0.25</v>
       </c>
       <c r="F41" s="30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G41" s="33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
@@ -1941,7 +1941,7 @@
         <v>33</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D42" s="35">
         <v>1</v>
@@ -1951,10 +1951,10 @@
         <v>0.1108</v>
       </c>
       <c r="F42" s="34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G42" s="37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
@@ -1974,7 +1974,7 @@
         <v>51</v>
       </c>
       <c r="G43" s="39" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
@@ -1982,7 +1982,7 @@
         <v>35</v>
       </c>
       <c r="C44" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44" s="35">
         <v>1</v>
@@ -1992,10 +1992,10 @@
         <v>0.83299999999999996</v>
       </c>
       <c r="F44" s="34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
@@ -2003,7 +2003,7 @@
         <v>36</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D45" s="35">
         <v>1</v>
@@ -2013,10 +2013,10 @@
         <v>0.38600000000000001</v>
       </c>
       <c r="F45" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G45" s="38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.2">
@@ -2033,10 +2033,10 @@
         <v>2.66</v>
       </c>
       <c r="F46" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="G46" s="38" t="s">
         <v>90</v>
-      </c>
-      <c r="G46" s="38" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.2">
@@ -2064,7 +2064,7 @@
         <v>39</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D48" s="49">
         <v>1</v>
@@ -2073,10 +2073,10 @@
         <v>10</v>
       </c>
       <c r="F48" s="51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G48" s="52" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
@@ -2094,7 +2094,7 @@
         <v>0.95</v>
       </c>
       <c r="F49" s="47" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G49" s="55" t="s">
         <v>59</v>
@@ -2104,7 +2104,7 @@
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
       <c r="D50" s="27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E50" s="28">
         <f>SUM(E11:E49)</f>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="52" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B52" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
@@ -2142,7 +2142,7 @@
         <v>44</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>19</v>
@@ -2156,7 +2156,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D54" s="35">
         <v>4</v>
@@ -2166,10 +2166,10 @@
         <v>4.58E-2</v>
       </c>
       <c r="F54" s="38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G54" s="38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.2">
@@ -2177,7 +2177,7 @@
         <v>2</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D55" s="1">
         <v>1</v>
@@ -2186,10 +2186,10 @@
         <v>9.2799999999999994</v>
       </c>
       <c r="F55" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.2">
@@ -2197,7 +2197,7 @@
         <v>3</v>
       </c>
       <c r="C56" s="44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D56" s="45">
         <v>1</v>
@@ -2207,10 +2207,10 @@
         <v>0.90500000000000003</v>
       </c>
       <c r="F56" s="47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G56" s="47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.2">
@@ -2231,14 +2231,14 @@
         <v>53</v>
       </c>
       <c r="G57" s="38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
       <c r="D58" s="27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E58" s="28">
         <f>SUM(E54:E57)</f>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="60" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B60" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="7"/>
@@ -2288,7 +2288,7 @@
         <v>1</v>
       </c>
       <c r="C62" s="34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D62" s="34">
         <v>1</v>
@@ -2298,10 +2298,10 @@
         <v>4.2699999999999995E-2</v>
       </c>
       <c r="F62" s="58" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G62" s="38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.2">
@@ -2309,20 +2309,20 @@
         <v>2</v>
       </c>
       <c r="C63" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D63" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E63" s="57">
         <f>8.95/10</f>
         <v>0.89499999999999991</v>
       </c>
       <c r="F63" s="58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G63" s="38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.2">
@@ -2330,20 +2330,20 @@
         <v>3</v>
       </c>
       <c r="C64" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" s="34" t="s">
         <v>79</v>
-      </c>
-      <c r="D64" s="34" t="s">
-        <v>80</v>
       </c>
       <c r="E64" s="57">
         <f>4.47/20</f>
         <v>0.22349999999999998</v>
       </c>
       <c r="F64" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="G64" s="38" t="s">
         <v>81</v>
-      </c>
-      <c r="G64" s="38" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.2">
@@ -2351,7 +2351,7 @@
         <v>4</v>
       </c>
       <c r="C65" s="34" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D65" s="34">
         <v>1</v>
@@ -2360,10 +2360,10 @@
         <v>3</v>
       </c>
       <c r="F65" s="58" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G65" s="59" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.2">
@@ -2371,7 +2371,7 @@
         <v>5</v>
       </c>
       <c r="C66" s="34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D66" s="34">
         <v>1</v>
@@ -2381,10 +2381,10 @@
         <v>4</v>
       </c>
       <c r="F66" s="58" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G66" s="59" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.2">
@@ -2392,7 +2392,7 @@
         <v>6</v>
       </c>
       <c r="C67" s="34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D67" s="34">
         <v>1</v>
@@ -2402,17 +2402,17 @@
         <v>5.96</v>
       </c>
       <c r="F67" s="58" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G67" s="59" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B68" s="20"/>
       <c r="C68" s="20"/>
       <c r="D68" s="60" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E68" s="28">
         <f>SUM(E62:E67)</f>
@@ -2441,7 +2441,7 @@
       <c r="B71" s="20"/>
       <c r="C71" s="20"/>
       <c r="D71" s="61" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E71" s="62">
         <f>E68+E58+E50</f>

</xml_diff>

<commit_message>
Updating the purchasing list
</commit_message>
<xml_diff>
--- a/Purchasing List.xlsx
+++ b/Purchasing List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5360" yWindow="440" windowWidth="28240" windowHeight="19420" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="460" windowWidth="28240" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="171">
   <si>
     <t>Link</t>
   </si>
@@ -56,15 +56,9 @@
     <t>CAP CER 1UF 50V Y5V 0805</t>
   </si>
   <si>
-    <t>CAP CER 10UF 6.3V X5R 0805</t>
-  </si>
-  <si>
     <t>CAP CER 0.1UF 50V X7R 0805</t>
   </si>
   <si>
-    <t>http://www.linear.com/product/LT3461A</t>
-  </si>
-  <si>
     <t>LT1807IS8#PBF</t>
   </si>
   <si>
@@ -92,9 +86,6 @@
     <t>6-pin connector</t>
   </si>
   <si>
-    <t>Digikey part number: WM5514-ND</t>
-  </si>
-  <si>
     <t>Digikey part number: S5440-ND</t>
   </si>
   <si>
@@ -125,12 +116,6 @@
     <t>Digikey Part Number: 399-8100-1-ND</t>
   </si>
   <si>
-    <t>Digikey Part Number: 587-1308-1-ND</t>
-  </si>
-  <si>
-    <t>Digikey Part Number: 490-1718-1-ND</t>
-  </si>
-  <si>
     <t>Digikey Part Number: 399-1170-1-ND</t>
   </si>
   <si>
@@ -188,9 +173,6 @@
     <t>LED Light Mounting Holders </t>
   </si>
   <si>
-    <t>http://sensl.com/estore/microfc-60035-smt/</t>
-  </si>
-  <si>
     <t>6x6mm SiPM MicroFC-60035-SMT</t>
   </si>
   <si>
@@ -203,9 +185,6 @@
     <t>OLED screen</t>
   </si>
   <si>
-    <t>https://www.elecrow.com/10pcs-2-layer-pcb.html</t>
-  </si>
-  <si>
     <t>Main PCB + SiPM PCB</t>
   </si>
   <si>
@@ -224,9 +203,6 @@
     <t>Rubber feet</t>
   </si>
   <si>
-    <t>Silicon bumper for feet</t>
-  </si>
-  <si>
     <t>Temperature sensor</t>
   </si>
   <si>
@@ -296,9 +272,6 @@
     <t>2 layer, 10cm x 10cm, 1.6mm thickness</t>
   </si>
   <si>
-    <t>Check Ebay or Amazon (example https://www.ebay.com/itm/131702108124)</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/uxcell-Plastic-Holder-Light-emitting-Lighting/dp/B00K859CGK/ref=sr_1_8?s=hi&amp;ie=UTF8&amp;qid=1511358277&amp;sr=1-8&amp;keywords=LED+holder</t>
   </si>
   <si>
@@ -323,9 +296,6 @@
     <t>TMP36 analog sensor</t>
   </si>
   <si>
-    <t>Check Ebay or Amazon (example: https://www.amazon.com/KOOKYE-Temperature-TMP36-Precision-Raspberry/dp/B01GH32AQU/ref=sr_1_1?ie=UTF8&amp;qid=1511358569&amp;sr=8-1&amp;keywords=tmp36 )</t>
-  </si>
-  <si>
     <t>Standoff threaded screws 0-80</t>
   </si>
   <si>
@@ -353,9 +323,6 @@
     <t>Aluminum Case</t>
   </si>
   <si>
-    <t>http://www.linear.com/purchase/LT1807</t>
-  </si>
-  <si>
     <t>Mouser Part Number: 595-CD74HC4050M96, https://pl.mouser.com/ProductDetail/Texas-Instruments/CD74HC4050M96/?qs=%2fha2pyFadui%2fKTy9HJ5lBx4ALNzSbmkwpijTk2ATsjJyZvwqthYvbg%3d%3d</t>
   </si>
   <si>
@@ -371,21 +338,12 @@
     <t>4 pin header for OLED</t>
   </si>
   <si>
-    <t>https://www.ebay.com/itm/200Pcs-Black-Silicone-Self-Adhesive-Rubber-Feet-Semicircle-Bumpers-Buffer-Pad-BE/192117515867?hash=item2cbb18a65b:g:gr4AAOSwWxNYt7qMdiameter/dp/B016GWHSBE/ref=pd_sim_60_1?_encoding=UTF8&amp;pd_rd_i=B016GWHSBE&amp;pd_rd_r=VR5P8R06S22F922NSZRT&amp;pd_rd_w=dl3hZ&amp;pd_rd_wg=INm00&amp;psc=1&amp;refRID=VR5P8R06S22F922NSZRT</t>
-  </si>
-  <si>
     <t>Other potential purchases</t>
   </si>
   <si>
     <t>microSD Card</t>
   </si>
   <si>
-    <t>We recommend anything above 200 Mb. Here is a 2Gb that we use.</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/product/B06Y3JGZSD/ref=oh_aui_detailpage_o05_s01?ie=UTF8&amp;psc=1</t>
-  </si>
-  <si>
     <t>Total:</t>
   </si>
   <si>
@@ -398,12 +356,6 @@
     <t>Coincidence Cable</t>
   </si>
   <si>
-    <t>https://www.amazon.com/dp/B0742CWDN8/ref=twister_B07429LJXQ?_encoding=UTF8&amp;psc=1</t>
-  </si>
-  <si>
-    <t>Recommend laser cutting: https://www.elecrow.com/5pcs-acrylic-laser-cutting-service.html</t>
-  </si>
-  <si>
     <t>10cm x 15cm x 2.5mm acrylic end plates.</t>
   </si>
   <si>
@@ -425,9 +377,6 @@
     <t>BNC Cable</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Hosa-BNC-59-103-75-ohm-Coax-Cable/dp/B000068OFB/ref=sr_1_4?ie=UTF8&amp;qid=1511362998&amp;sr=8-4&amp;keywords=bnc+cable</t>
-  </si>
-  <si>
     <t>3 feet BNC cable for testing.</t>
   </si>
   <si>
@@ -437,9 +386,6 @@
     <t>Note 2: We try and include a link in the form of the part number for each website</t>
   </si>
   <si>
-    <t xml:space="preserve">Note 3: We purhace our components in bulk (as required by several of the components). The price/unit was determined by purchasing 100 of each component. </t>
-  </si>
-  <si>
     <t>47uH inductor</t>
   </si>
   <si>
@@ -461,9 +407,6 @@
     <t>Digikey Part Number: 311-0.0ARCT-ND</t>
   </si>
   <si>
-    <t>You want something that peaks in the 420nm range.</t>
-  </si>
-  <si>
     <t>249 Ohm resistor</t>
   </si>
   <si>
@@ -503,9 +446,6 @@
     <t>CAP CER 20nF 50V X7R 0805</t>
   </si>
   <si>
-    <t>Digikey Part Number: 1276-2472-1-ND</t>
-  </si>
-  <si>
     <t>SMT SMD Cell Phone TF Micro SD Memory Card Slot Holder Sockets</t>
   </si>
   <si>
@@ -518,12 +458,6 @@
     <t>CAP CER 10000PF 50V X7R 0805</t>
   </si>
   <si>
-    <t>490-1664-1-ND</t>
-  </si>
-  <si>
-    <t>Digikey Part Number: 490-1664-1-ND</t>
-  </si>
-  <si>
     <t>10nF capacitor</t>
   </si>
   <si>
@@ -533,8 +467,41 @@
     <t>1/8" Hex Size, 7/16"" Length, 0-80 Thread Size</t>
   </si>
   <si>
+    <t>Digikey Part Number: 478-10429-6-ND</t>
+  </si>
+  <si>
+    <t>Digikey Part Number: 1276-6470-1-ND</t>
+  </si>
+  <si>
+    <t>Digikey Part Number: 276-2563-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 10.0V X5R 0805</t>
+  </si>
+  <si>
+    <t>Digikey Part Number: 1276-6456-1-ND</t>
+  </si>
+  <si>
+    <t>Digikey part number: A97555-ND (old version WM5514-ND)</t>
+  </si>
+  <si>
+    <t>https://www.analog.com/en/products/lt3461a.html#product-samplebuy</t>
+  </si>
+  <si>
+    <t>https://www.analog.com/en/products/lt1807.html#product-samplebuy</t>
+  </si>
+  <si>
+    <t>Check Ebay or Amazon (example https://www.amazon.com/ELEGOO-Arduino-ATmega328P-Without-Compatible/dp/B0713XK923/ref=sr_1_4?keywords=arduino+nano&amp;qid=1578433105&amp;sr=8-4)</t>
+  </si>
+  <si>
+    <t>Check Ebay or Amazon (example: https://www.amazon.com/KOOKYE-Temperature-TMP36-Precision-Raspberry/dp/B01GH32AQU/ref=sxts_sxwds-bia?crid=2SXPT5QDNERXY&amp;cv_ct_cx=tmp36+temperature+sensor&amp;keywords=tmp36+temperature+sensor&amp;pd_rd_i=B01GH32AQU&amp;pd_rd_r=dd854d23-d9df-41d3-ac9f-bcbe484cf6e0&amp;pd_rd_w=sjoTX&amp;pd_rd_wg=8Xbk1&amp;pf_rd_p=1cb3f32a-ccfd-479b-8a13-b22f56c942c6&amp;pf_rd_r=KN5GH2PHK0PDN9EQ7EH8&amp;psc=1&amp;qid=1578433136&amp;sprefix=tmp%2Caps%2C135 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note7: Ebay is often cheap than amazon. But the products change names regularly, so I won't include links to Ebay. </t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Check Ebay or Amazon (example: https://www.ebay.com/itm/122441882218) </t>
+      <t xml:space="preserve">Check Ebay or Amazon (example: https://www.amazon.com/Dorhea-Display-SSD1306-Self-Luminous-Raspberry/dp/B07FK8GB8T/ref=sr_1_4?keywords=oled%2B96&amp;qid=1578433279&amp;sr=8-4&amp;th=1) </t>
     </r>
     <r>
       <rPr>
@@ -542,8 +509,44 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>NOTE: VCC NEEDS TO BE THE 4th PIN ON THE OLED, IT CANNOT BE THE GND PIN. SOME MANUFACTURERS SWAP THE PINS.</t>
+      <t>NOTE: VCC NEEDS TO BE THE 4th PIN ON THE OLED (on the left side), the left most pin is GND on half of the screens out there. SOME MANUFACTURERS SWAP THE PINS.</t>
     </r>
+  </si>
+  <si>
+    <t>Note 8: Half of the OLED screens out there have VCC and GND reversed. We want an OLED screen with the VCC pin as the left most pin, not the second left-most pin.</t>
+  </si>
+  <si>
+    <t>Mouser part Number: 863-MFC60035SMTTR1 (https://www.mouser.com/ProductDetail/ON-Semiconductor/MICROFC-60035-SMT-TR1?qs=byeeYqUIh0MxSRIaBcfS6g%3D%3D)</t>
+  </si>
+  <si>
+    <t>Ebay, or find your own. You want 5x5x1 cm3 and a peak emission at 420nm.  (https://www.ebay.com/itm/Bicron-BC408-Plastic-Scintillator-5x5x1-cm-for-CosmicWatch-Muon-Detector-Project/263355405917?epid=2044114641&amp;hash=item3d5134965d:g:XxsAAOSwSW5cWxPb)</t>
+  </si>
+  <si>
+    <t>https://www.elecrow.com/pcb-manufacturing.html</t>
+  </si>
+  <si>
+    <t>Silicon bumper for feet, 8x2 mm</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/200PC-Self-Adhesive-Silicone-Feet-Bumpers-Stop-Clear-Cabinet-Door-Buffer-Pads-US/153282008606?hash=item23b051d61e:g:L~EAAOSw1vxcdcKE</t>
+  </si>
+  <si>
+    <t>https://www.elecrow.com/acrylic-cutting.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We recommend anything above 200 Mb. </t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Kingston-microSDHC-Memory-SDC4-8GBET/dp/B00200K1TS/ref=sr_1_4?keywords=2gb+micro+sd+card&amp;qid=1578433784&amp;s=electronics&amp;sr=1-4</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Seadream-4-Pole-Stereo-Headset-Extension/dp/B017PT8XX4/ref=sr_1_10?keywords=3.5mm+audio+cable+6inches&amp;qid=1578433918&amp;sr=8-10</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Hosa-BNC-59-103-75-Ohm-Coax-Cable/dp/B000068OFB/ref=sxin_2_ac_d_pm?ac_md=1-0-VW5kZXIgJDEw-ac_d_pm&amp;cv_ct_cx=bnc+cable&amp;keywords=bnc+cable&amp;pd_rd_i=B000068OFB&amp;pd_rd_r=1cda2177-58fe-4ab1-9b9b-8d25fb08ecd7&amp;pd_rd_w=T8pUo&amp;pd_rd_wg=aacgH&amp;pf_rd_p=709d2064-e546-4799-9e66-b352ea89951f&amp;pf_rd_r=7JTRZ5RG5EVZGCSKHM2J&amp;psc=1&amp;qid=1578433945&amp;s=electronics</t>
+  </si>
+  <si>
+    <t>Note 3: We purhace our components in bulk (as required by several of the components). The price/unit was determined by purchasing 100 of each component.  If you purchase a single unit, the price is probably ~200USD.</t>
   </si>
 </sst>
 </file>
@@ -1184,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G73"/>
+  <dimension ref="B1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="114" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1202,20 +1205,20 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B1" s="20" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="C1" s="20"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="20" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="C2" s="20"/>
       <c r="F2" s="20"/>
     </row>
     <row r="3" spans="2:7" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>137</v>
+        <v>170</v>
       </c>
       <c r="C3" s="20"/>
       <c r="F3" s="20"/>
@@ -1223,1224 +1226,1221 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="20" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="C4" s="20"/>
       <c r="G4" s="21"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="C5" s="20"/>
-      <c r="G5" s="56" t="s">
-        <v>163</v>
-      </c>
+      <c r="G5" s="56"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="20" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="F6" s="56"/>
-      <c r="G6" s="56" t="s">
-        <v>164</v>
-      </c>
+      <c r="G6" s="56"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="20"/>
+      <c r="B7" s="20" t="s">
+        <v>157</v>
+      </c>
       <c r="F7" s="56"/>
-      <c r="G7" s="21"/>
-    </row>
-    <row r="8" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="G7" s="56"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" s="56"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="E10" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="8">
-        <v>1</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" s="9">
-        <v>5</v>
-      </c>
-      <c r="E10" s="22">
-        <f>0.0071*D10</f>
-        <v>3.5500000000000004E-2</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="D11" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E11" s="22">
-        <f>0.0088 *D11</f>
-        <v>3.5200000000000002E-2</v>
+        <f>0.0071*D11</f>
+        <v>3.5500000000000004E-2</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>146</v>
+        <v>40</v>
       </c>
       <c r="D12" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" s="22">
         <f>0.0088 *D12</f>
-        <v>1.7600000000000001E-2</v>
+        <v>3.5200000000000002E-2</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>147</v>
+        <v>18</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>148</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="D13" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E13" s="22">
         <f>0.0088 *D13</f>
-        <v>3.5200000000000002E-2</v>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>3</v>
+        <v>128</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>27</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D14" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" s="22">
-        <f>0.0088*D14</f>
-        <v>4.4000000000000004E-2</v>
+        <f>0.0088 *D14</f>
+        <v>3.5200000000000002E-2</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>149</v>
+        <v>36</v>
       </c>
       <c r="D15" s="9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15" s="22">
-        <f>0.0088 *D15</f>
-        <v>1.7600000000000001E-2</v>
+        <f>0.0088*D15</f>
+        <v>4.4000000000000004E-2</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>151</v>
+        <v>1</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>150</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="D16" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E16" s="22">
-        <f>0.0088*D16</f>
-        <v>2.64E-2</v>
+        <f>0.0088 *D16</f>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>4</v>
+        <v>132</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>28</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D17" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17" s="22">
         <f>0.0088*D17</f>
-        <v>1.7600000000000001E-2</v>
+        <v>2.64E-2</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
       <c r="D18" s="9">
         <v>2</v>
       </c>
       <c r="E18" s="22">
-        <f>0.0267 *D18</f>
-        <v>5.3400000000000003E-2</v>
+        <f>0.0088*D18</f>
+        <v>1.7600000000000001E-2</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>153</v>
+        <v>2</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>154</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>82</v>
+        <v>133</v>
       </c>
       <c r="D19" s="9">
         <v>2</v>
       </c>
       <c r="E19" s="22">
-        <f>0.0248 *D19</f>
-        <v>4.9599999999999998E-2</v>
+        <f>0.0267 *D19</f>
+        <v>5.3400000000000003E-2</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>7</v>
+        <v>134</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>31</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="8">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D20" s="9">
         <v>2</v>
       </c>
       <c r="E20" s="22">
-        <f>0.1092 *D20</f>
-        <v>0.21840000000000001</v>
+        <f>0.0248 *D20</f>
+        <v>4.9599999999999998E-2</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="8">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D21" s="8">
-        <v>6</v>
-      </c>
-      <c r="E21" s="23">
-        <f>0.0158*D21</f>
-        <v>9.4800000000000009E-2</v>
+        <v>75</v>
+      </c>
+      <c r="D21" s="9">
+        <v>2</v>
+      </c>
+      <c r="E21" s="22">
+        <f>0.1092 *D21</f>
+        <v>0.21840000000000001</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>158</v>
+        <v>8</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="8">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" s="9">
-        <v>4</v>
-      </c>
-      <c r="E22" s="22">
-        <f>0.0248*D22</f>
-        <v>9.9199999999999997E-2</v>
+        <v>138</v>
+      </c>
+      <c r="D22" s="8">
+        <v>6</v>
+      </c>
+      <c r="E22" s="23">
+        <f>0.0158*D22</f>
+        <v>9.4800000000000009E-2</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>11</v>
+        <v>139</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>35</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="8">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D23" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E23" s="22">
-        <f>0.038*D23</f>
-        <v>0.11399999999999999</v>
+        <f>0.0248*D23</f>
+        <v>9.9199999999999997E-2</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="8">
+        <v>14</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="9">
+        <v>3</v>
+      </c>
+      <c r="E24" s="22">
+        <f>0.038*D24</f>
+        <v>0.11399999999999999</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="8">
         <v>15</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D24" s="9">
+      <c r="C25" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D25" s="9">
         <v>4</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E25" s="22">
         <f>0.0335</f>
         <v>3.3500000000000002E-2</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="8">
-        <v>16</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="9">
-        <v>3</v>
-      </c>
-      <c r="E25" s="22">
-        <f>0.0413*D25</f>
-        <v>0.12390000000000001</v>
-      </c>
       <c r="F25" s="10" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>34</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="8">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="D26" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26" s="22">
-        <f>0.0536*D26</f>
-        <v>0.1072</v>
+        <f>0.0413*D26</f>
+        <v>0.12390000000000001</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="8">
+        <v>17</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="9">
+        <v>2</v>
+      </c>
+      <c r="E27" s="22">
+        <f>0.0536*D27</f>
+        <v>0.1072</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="8">
         <v>18</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D27" s="9">
-        <v>1</v>
-      </c>
-      <c r="E27" s="22">
+      <c r="C28" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="22">
         <f>0.2226</f>
         <v>0.22259999999999999</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F28" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="8">
+      <c r="G28" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="8">
         <v>19</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="9">
+      <c r="C29" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="9">
         <v>2</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E29" s="22">
         <f>0.1627 *2</f>
         <v>0.32540000000000002</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F29" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G28" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="8">
+      <c r="G29" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="8">
         <v>20</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D29" s="9">
-        <v>1</v>
-      </c>
-      <c r="E29" s="22">
+      <c r="C30" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="9">
+        <v>1</v>
+      </c>
+      <c r="E30" s="22">
         <f>0.4</f>
         <v>0.4</v>
       </c>
-      <c r="F29" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="8">
+      <c r="F30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="8">
         <v>21</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="9">
-        <v>1</v>
-      </c>
-      <c r="E30" s="22">
+      <c r="C31" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="9">
+        <v>1</v>
+      </c>
+      <c r="E31" s="22">
         <f>0.4069</f>
         <v>0.40689999999999998</v>
       </c>
-      <c r="F30" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="8">
+      <c r="F31" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="8">
         <v>22</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="9">
-        <v>1</v>
-      </c>
-      <c r="E31" s="22">
+      <c r="C32" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="9">
+        <v>1</v>
+      </c>
+      <c r="E32" s="22">
         <f>0.4509</f>
         <v>0.45090000000000002</v>
       </c>
-      <c r="F31" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="8">
+      <c r="F32" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="8">
         <v>23</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="9">
-        <v>1</v>
-      </c>
-      <c r="E32" s="22">
+      <c r="C33" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="9">
+        <v>1</v>
+      </c>
+      <c r="E33" s="22">
         <f>0.1862</f>
         <v>0.1862</v>
       </c>
-      <c r="F32" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="10" t="s">
+      <c r="F33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="8">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="8">
-        <v>24</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D33" s="18">
-        <v>1</v>
-      </c>
-      <c r="E33" s="24">
+      <c r="C34" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="18">
+        <v>1</v>
+      </c>
+      <c r="E34" s="24">
         <f>0.8906</f>
         <v>0.89059999999999995</v>
       </c>
-      <c r="F33" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="8">
+      <c r="F34" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="8">
         <v>25</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D34" s="9">
-        <v>1</v>
-      </c>
-      <c r="E34" s="22">
+      <c r="C35" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="9">
+        <v>1</v>
+      </c>
+      <c r="E35" s="22">
         <f>1.6727</f>
         <v>1.6727000000000001</v>
       </c>
-      <c r="F34" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="8">
+      <c r="F35" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="8">
         <v>26</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D35" s="9">
-        <v>1</v>
-      </c>
-      <c r="E35" s="22">
+      <c r="C36" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="9">
+        <v>1</v>
+      </c>
+      <c r="E36" s="22">
         <f>0.1973</f>
         <v>0.1973</v>
       </c>
-      <c r="F35" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="8">
+      <c r="F36" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37" s="8">
         <v>27</v>
       </c>
-      <c r="C36" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="12">
+      <c r="C37" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="12">
         <v>2</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E37" s="25">
         <f>0.33*2</f>
         <v>0.66</v>
       </c>
-      <c r="F36" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="8">
+      <c r="F37" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B38" s="8">
         <v>28</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D37" s="12">
+      <c r="C38" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="12">
         <v>4</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E38" s="25">
         <f>9.01/100*4</f>
         <v>0.3604</v>
       </c>
-      <c r="F37" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="8">
+      <c r="F38" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B39" s="8">
         <v>29</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="12">
+      <c r="C39" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="12">
         <v>4</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E39" s="25">
         <f>6.95/50*2</f>
         <v>0.27800000000000002</v>
       </c>
-      <c r="F38" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="8">
-        <v>30</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="D39" s="15">
-        <v>1</v>
-      </c>
-      <c r="E39" s="26">
-        <v>2</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>12</v>
+      <c r="F39" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="8">
+        <v>30</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="15">
+        <v>1</v>
+      </c>
+      <c r="E40" s="26">
+        <v>2</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="8">
         <v>31</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D40" s="15">
-        <v>1</v>
-      </c>
-      <c r="E40" s="26">
+      <c r="C41" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="15">
+        <v>1</v>
+      </c>
+      <c r="E41" s="26">
         <f>3.75</f>
         <v>3.75</v>
       </c>
-      <c r="F40" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="8">
-        <v>32</v>
-      </c>
-      <c r="C41" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="31">
-        <v>1</v>
-      </c>
-      <c r="E41" s="32">
-        <v>0.25</v>
-      </c>
-      <c r="F41" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="G41" s="33" t="s">
-        <v>110</v>
+      <c r="F41" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="8">
+        <v>32</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42" s="31">
+        <v>1</v>
+      </c>
+      <c r="E42" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="F42" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="G42" s="33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B43" s="8">
         <v>33</v>
       </c>
-      <c r="C42" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="35">
-        <v>1</v>
-      </c>
-      <c r="E42" s="36">
+      <c r="C43" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" s="35">
+        <v>1</v>
+      </c>
+      <c r="E43" s="36">
         <f>5.54/50</f>
         <v>0.1108</v>
       </c>
-      <c r="F42" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="G42" s="37" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B43" s="8">
-        <v>34</v>
-      </c>
-      <c r="C43" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="35">
-        <v>1</v>
-      </c>
-      <c r="E43" s="36">
-        <v>2.246</v>
-      </c>
-      <c r="F43" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="G43" s="39" t="s">
-        <v>90</v>
+      <c r="F43" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="G43" s="37" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44" s="8">
+        <v>34</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="35">
+        <v>1</v>
+      </c>
+      <c r="E44" s="36">
+        <v>2.246</v>
+      </c>
+      <c r="F44" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="G44" s="39" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B45" s="8">
         <v>35</v>
       </c>
-      <c r="C44" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="D44" s="35">
-        <v>1</v>
-      </c>
-      <c r="E44" s="36">
+      <c r="C45" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="35">
+        <v>1</v>
+      </c>
+      <c r="E45" s="36">
         <f>8.33/10</f>
         <v>0.83299999999999996</v>
       </c>
-      <c r="F44" s="34" t="s">
-        <v>98</v>
-      </c>
-      <c r="G44" s="34" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B45" s="8">
+      <c r="F45" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="G45" s="34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B46" s="8">
         <v>36</v>
       </c>
-      <c r="C45" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="D45" s="35">
-        <v>1</v>
-      </c>
-      <c r="E45" s="36">
+      <c r="C46" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" s="35">
+        <v>1</v>
+      </c>
+      <c r="E46" s="36">
         <f>3.86/10</f>
         <v>0.38600000000000001</v>
       </c>
-      <c r="F45" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="G45" s="38" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B46" s="8">
-        <v>37</v>
-      </c>
-      <c r="C46" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="D46" s="35">
-        <v>1</v>
-      </c>
-      <c r="E46" s="36">
-        <v>2.66</v>
-      </c>
       <c r="F46" s="38" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="G46" s="38" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47" s="8">
-        <v>38</v>
-      </c>
-      <c r="C47" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="41">
-        <v>1</v>
-      </c>
-      <c r="E47" s="42">
-        <v>48</v>
-      </c>
-      <c r="F47" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="G47" s="43" t="s">
-        <v>54</v>
+        <v>37</v>
+      </c>
+      <c r="C47" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="35">
+        <v>1</v>
+      </c>
+      <c r="E47" s="36">
+        <v>2.66</v>
+      </c>
+      <c r="F47" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G47" s="38" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48" s="8">
-        <v>39</v>
-      </c>
-      <c r="C48" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="D48" s="49">
-        <v>1</v>
-      </c>
-      <c r="E48" s="50">
-        <v>10</v>
-      </c>
-      <c r="F48" s="51" t="s">
-        <v>69</v>
-      </c>
-      <c r="G48" s="52" t="s">
-        <v>145</v>
+        <v>38</v>
+      </c>
+      <c r="C48" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" s="41">
+        <v>1</v>
+      </c>
+      <c r="E48" s="42">
+        <v>48</v>
+      </c>
+      <c r="F48" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="G48" s="43" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="8">
+        <v>39</v>
+      </c>
+      <c r="C49" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="49">
+        <v>1</v>
+      </c>
+      <c r="E49" s="50">
+        <v>10</v>
+      </c>
+      <c r="F49" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="G49" s="52" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B50" s="8">
         <v>40</v>
       </c>
-      <c r="C49" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="45">
-        <v>1</v>
-      </c>
-      <c r="E49" s="46">
+      <c r="C50" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" s="45">
+        <v>1</v>
+      </c>
+      <c r="E50" s="46">
         <f>9.5/10</f>
         <v>0.95</v>
       </c>
-      <c r="F49" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="G49" s="55" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E50" s="28">
-        <f>SUM(E11:E49)</f>
-        <v>78.324399999999997</v>
-      </c>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
+      <c r="F50" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="G50" s="55" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
+      <c r="D51" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E51" s="28">
+        <f>SUM(E12:E50)</f>
+        <v>78.324399999999997</v>
+      </c>
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
     </row>
-    <row r="52" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B52" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B53" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C53" s="3" t="s">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+    </row>
+    <row r="53" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="B53" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G53" s="3" t="s">
+      <c r="E54" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B54" s="34">
-        <v>1</v>
-      </c>
-      <c r="C54" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="D54" s="35">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B55" s="34">
+        <v>1</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D55" s="35">
         <v>4</v>
       </c>
-      <c r="E54" s="36">
+      <c r="E55" s="36">
         <f>2.29/200*4</f>
         <v>4.58E-2</v>
       </c>
-      <c r="F54" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="G54" s="38" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B55" s="1">
+      <c r="F55" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="G55" s="59" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B56" s="1">
         <v>2</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D55" s="1">
-        <v>1</v>
-      </c>
-      <c r="E55" s="29">
+      <c r="C56" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1</v>
+      </c>
+      <c r="E56" s="29">
         <v>9.2799999999999994</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B56" s="44">
+      <c r="F56" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B57" s="44">
         <v>3</v>
       </c>
-      <c r="C56" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="D56" s="45">
-        <v>1</v>
-      </c>
-      <c r="E56" s="46">
+      <c r="C57" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" s="45">
+        <v>1</v>
+      </c>
+      <c r="E57" s="46">
         <f>9.05/10</f>
         <v>0.90500000000000003</v>
       </c>
-      <c r="F56" s="47" t="s">
-        <v>126</v>
-      </c>
-      <c r="G56" s="47" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B57" s="34">
+      <c r="F57" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="G57" s="47" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B58" s="34">
         <v>4</v>
       </c>
-      <c r="C57" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D57" s="35">
-        <v>1</v>
-      </c>
-      <c r="E57" s="36">
+      <c r="C58" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D58" s="35">
+        <v>1</v>
+      </c>
+      <c r="E58" s="36">
         <f>7.7/50</f>
         <v>0.154</v>
       </c>
-      <c r="F57" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="G57" s="38" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="E58" s="28">
-        <f>SUM(E54:E57)</f>
-        <v>10.384799999999998</v>
-      </c>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
+      <c r="F58" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="G58" s="38" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="53"/>
+      <c r="D59" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" s="28">
+        <f>SUM(E55:E58)</f>
+        <v>10.384799999999998</v>
+      </c>
       <c r="F59" s="20"/>
       <c r="G59" s="20"/>
     </row>
-    <row r="60" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B60" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B61" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C61" s="3" t="s">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+    </row>
+    <row r="61" spans="2:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="B61" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" s="6"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B62" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G61" s="3" t="s">
+      <c r="E62" s="3"/>
+      <c r="F62" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G62" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B62" s="34">
-        <v>1</v>
-      </c>
-      <c r="C62" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="D62" s="34">
-        <v>1</v>
-      </c>
-      <c r="E62" s="57">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B63" s="34">
+        <v>1</v>
+      </c>
+      <c r="C63" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D63" s="34">
+        <v>1</v>
+      </c>
+      <c r="E63" s="57">
         <f>8.54/200</f>
         <v>4.2699999999999995E-2</v>
       </c>
-      <c r="F62" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="G62" s="38" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B63" s="34">
+      <c r="F63" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="G63" s="38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B64" s="34">
         <v>2</v>
       </c>
-      <c r="C63" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D63" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="E63" s="57">
+      <c r="C64" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D64" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" s="57">
         <f>8.95/10</f>
         <v>0.89499999999999991</v>
       </c>
-      <c r="F63" s="58" t="s">
-        <v>77</v>
-      </c>
-      <c r="G63" s="38" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B64" s="34">
+      <c r="F64" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="G64" s="38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B65" s="34">
         <v>3</v>
       </c>
-      <c r="C64" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="D64" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="E64" s="57">
+      <c r="C65" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E65" s="57">
         <f>4.47/20</f>
         <v>0.22349999999999998</v>
       </c>
-      <c r="F64" s="58" t="s">
-        <v>80</v>
-      </c>
-      <c r="G64" s="38" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B65" s="34">
-        <v>4</v>
-      </c>
-      <c r="C65" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="D65" s="34">
-        <v>1</v>
-      </c>
-      <c r="E65" s="57">
-        <v>3</v>
-      </c>
       <c r="F65" s="58" t="s">
-        <v>118</v>
-      </c>
-      <c r="G65" s="59" t="s">
-        <v>119</v>
+        <v>72</v>
+      </c>
+      <c r="G65" s="38" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B66" s="34">
+        <v>4</v>
+      </c>
+      <c r="C66" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="D66" s="34">
+        <v>1</v>
+      </c>
+      <c r="E66" s="57">
+        <v>3</v>
+      </c>
+      <c r="F66" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="G66" s="59" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B67" s="34">
         <v>5</v>
       </c>
-      <c r="C66" s="34" t="s">
-        <v>123</v>
-      </c>
-      <c r="D66" s="34">
-        <v>1</v>
-      </c>
-      <c r="E66" s="57">
+      <c r="C67" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D67" s="34">
+        <v>1</v>
+      </c>
+      <c r="E67" s="57">
         <f>8/2</f>
         <v>4</v>
       </c>
-      <c r="F66" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="G66" s="59" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B67" s="34">
+      <c r="F67" s="58" t="s">
+        <v>112</v>
+      </c>
+      <c r="G67" s="59" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B68" s="34">
         <v>6</v>
       </c>
-      <c r="C67" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="D67" s="34">
-        <v>1</v>
-      </c>
-      <c r="E67" s="57">
+      <c r="C68" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D68" s="34">
+        <v>1</v>
+      </c>
+      <c r="E68" s="57">
         <f>5.96</f>
         <v>5.96</v>
       </c>
-      <c r="F67" s="58" t="s">
-        <v>134</v>
-      </c>
-      <c r="G67" s="59" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B68" s="20"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="60" t="s">
-        <v>120</v>
-      </c>
-      <c r="E68" s="28">
-        <f>SUM(E62:E67)</f>
-        <v>14.121200000000002</v>
-      </c>
-      <c r="F68" s="20"/>
-      <c r="G68" s="20"/>
+      <c r="F68" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="G68" s="59" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="69" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B69" s="20"/>
       <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
+      <c r="D69" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="E69" s="28">
+        <f>SUM(E63:E68)</f>
+        <v>14.121200000000002</v>
+      </c>
       <c r="F69" s="20"/>
       <c r="G69" s="20"/>
     </row>
@@ -2452,24 +2452,24 @@
       <c r="F70" s="20"/>
       <c r="G70" s="20"/>
     </row>
-    <row r="71" spans="2:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B71" s="20"/>
       <c r="C71" s="20"/>
-      <c r="D71" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="E71" s="62">
-        <f>E68+E58+E50</f>
-        <v>102.8304</v>
-      </c>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
       <c r="F71" s="20"/>
       <c r="G71" s="20"/>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:7" ht="19" x14ac:dyDescent="0.25">
       <c r="B72" s="20"/>
       <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
+      <c r="D72" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="E72" s="62">
+        <f>E69+E59+E51</f>
+        <v>102.8304</v>
+      </c>
       <c r="F72" s="20"/>
       <c r="G72" s="20"/>
     </row>
@@ -2481,13 +2481,21 @@
       <c r="F73" s="20"/>
       <c r="G73" s="20"/>
     </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B74" s="20"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="20"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G42" r:id="rId1"/>
-    <hyperlink ref="G65" r:id="rId2"/>
-    <hyperlink ref="G49" r:id="rId3"/>
+    <hyperlink ref="G43" r:id="rId1"/>
+    <hyperlink ref="G66" r:id="rId2" display="https://www.amazon.com/gp/product/B06Y3JGZSD/ref=oh_aui_detailpage_o05_s01?ie=UTF8&amp;psc=1"/>
+    <hyperlink ref="G50" r:id="rId3" display="https://www.elecrow.com/10pcs-2-layer-pcb.html"/>
     <hyperlink ref="G67" r:id="rId4" display="https://www.amazon.com/dp/B0742CWDN8/ref=twister_B07429LJXQ?_encoding=UTF8&amp;psc=1"/>
-    <hyperlink ref="G66" r:id="rId5"/>
+    <hyperlink ref="G55" r:id="rId5" display="https://www.ebay.com/itm/200Pcs-Black-Silicone-Self-Adhesive-Rubber-Feet-Semicircle-Bumpers-Buffer-Pad"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>